<commit_message>
docs: update matriz 5W2H
</commit_message>
<xml_diff>
--- a/ProjetoVitrineVirtural/Documentation/Artefatos-final/5W2H.xlsx
+++ b/ProjetoVitrineVirtural/Documentation/Artefatos-final/5W2H.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus Gomes\Desktop\área de trabalho\Desenvolvedor\ADS FATEC\4- Semestre\Engenharia de Software III\Projeto Vitrine Virtural\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matheus Gomes\Desktop\área de trabalho\Desenvolvedor\ADS FATEC\4- Semestre\Engenharia de Software III\ProjetoVitrineVirtural\Documentation\Artefatos-final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBE5760-B60E-4338-8363-BD94E481BBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC0417-7141-4AFB-B464-2B105E8E87E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-8340" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -259,7 +259,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF00FF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,6 +342,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -359,9 +362,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,16 +667,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -801,16 +801,16 @@
       <c r="I5" s="6"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -894,16 +894,16 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -999,16 +999,16 @@
       <c r="H16" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
@@ -1073,66 +1073,66 @@
       <c r="H22" s="10"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="16" t="s">
+      <c r="G25" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="A26" s="17">
         <v>1</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="18" t="s">
         <v>35</v>
       </c>
       <c r="I26" s="11" t="s">
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
+      <c r="A27" s="12">
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1166,16 +1166,16 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -1282,23 +1282,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="53114aab-23d5-4c61-b27d-c52731a736fe" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BD4E946A9A0AE84E9DA87CDA95DB11DF" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3730b19e1d9f6b6e7fedbc6fff5eacf2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="53114aab-23d5-4c61-b27d-c52731a736fe" xmlns:ns4="6c9fa380-4f98-48aa-91bb-f1e00e7e67c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="223ebba38945585d58b3fe219b67c875" ns3:_="" ns4:_="">
     <xsd:import namespace="53114aab-23d5-4c61-b27d-c52731a736fe"/>
@@ -1493,10 +1476,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="53114aab-23d5-4c61-b27d-c52731a736fe" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82E6A921-1D81-417A-BB5E-A204CEC781EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{318F9F2F-0661-4F96-B7DA-04F8AE74FD2B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="53114aab-23d5-4c61-b27d-c52731a736fe"/>
+    <ds:schemaRef ds:uri="6c9fa380-4f98-48aa-91bb-f1e00e7e67c7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1519,20 +1530,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{318F9F2F-0661-4F96-B7DA-04F8AE74FD2B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82E6A921-1D81-417A-BB5E-A204CEC781EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="53114aab-23d5-4c61-b27d-c52731a736fe"/>
-    <ds:schemaRef ds:uri="6c9fa380-4f98-48aa-91bb-f1e00e7e67c7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>